<commit_message>
complete sitting arrangment pushed
</commit_message>
<xml_diff>
--- a/static/seating.xlsx
+++ b/static/seating.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="153">
   <si>
     <t>ALADE-AKINYEMI, LOLU</t>
   </si>
@@ -273,6 +273,216 @@
   </si>
   <si>
     <t>OGUNKUNLE, AANU OLAOLUWA</t>
+  </si>
+  <si>
+    <t>EDUN, OLUWOLE ADEDAYO</t>
+  </si>
+  <si>
+    <t>ALODE, ADEWUNMI AJIKE</t>
+  </si>
+  <si>
+    <t>AKINTOLU, KAYODE IBRAHIM</t>
+  </si>
+  <si>
+    <t>OGUNYINKA, OLAKUNLE SUNDAY</t>
+  </si>
+  <si>
+    <t>AYEKPESA, EGHEORIARERE MIGHTY</t>
+  </si>
+  <si>
+    <t>OLAYEMI, ABIODUN OLALEKAN</t>
+  </si>
+  <si>
+    <t>UKPEBOR, THOMPSON OSALEN</t>
+  </si>
+  <si>
+    <t>KUPOLATI, ELIJAH OLUFEMI</t>
+  </si>
+  <si>
+    <t>EDWARDS, MARK REGINALD</t>
+  </si>
+  <si>
+    <t>IWENDI, PETER NDUBUISI</t>
+  </si>
+  <si>
+    <t>ADAMU, FRANCIS KAYODE</t>
+  </si>
+  <si>
+    <t>BAKARE, ADEKUNLE GANIYU</t>
+  </si>
+  <si>
+    <t>AZEEZ-ENILOLOBO, MOSUNMOLA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">KAREEM, GANIYU SALAM BABATUNDE </t>
+  </si>
+  <si>
+    <t>MILAD, HANNA AZIZ HANNA</t>
+  </si>
+  <si>
+    <t>YAKUBU, ALIU YUSUF</t>
+  </si>
+  <si>
+    <t>JIMOH, TAIWO LUQMAN</t>
+  </si>
+  <si>
+    <t>MOSES, OLUYOMI OLULEKE</t>
+  </si>
+  <si>
+    <t>ADEWUYI, OLUSOJI</t>
+  </si>
+  <si>
+    <t>OMOTUNDE, ALAYODE MOBOLAJI</t>
+  </si>
+  <si>
+    <t>YERRABELLY, VENKAT NARSIMHA RAO</t>
+  </si>
+  <si>
+    <t>OSAGIE, EKPEN OBA</t>
+  </si>
+  <si>
+    <t>ODENIYI, AKINOLA TEMITOPE</t>
+  </si>
+  <si>
+    <t>John Olusesan AJALA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adeyemi Ariyo </t>
+  </si>
+  <si>
+    <t>DICKSON IMARENEZOR AZEMHETA</t>
+  </si>
+  <si>
+    <t>SALAKO, JAMIU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OJIEH, LAMBERT UGOCHUKWU </t>
+  </si>
+  <si>
+    <t>MADAKI, MUSA BUNGUM</t>
+  </si>
+  <si>
+    <t>ODIMAYO, OLUROTIMI</t>
+  </si>
+  <si>
+    <t>MADOJUTIMI, OLUFUNKE</t>
+  </si>
+  <si>
+    <t>OLORODE, MORENIKEJI OYEPERO</t>
+  </si>
+  <si>
+    <t>UNUKPO, PETER AGHOGHO</t>
+  </si>
+  <si>
+    <t>SALAMI, GREGORY IMOUKHUEDE</t>
+  </si>
+  <si>
+    <t>SOBOLA, AUGUSTINA IFEYINWA</t>
+  </si>
+  <si>
+    <t>ARAGHO, JEMINE MICHAEL</t>
+  </si>
+  <si>
+    <t>ADEBOYE, OWOYEMI AZEEZ</t>
+  </si>
+  <si>
+    <t>ABOSEDE, LANRE AUGUSTINE</t>
+  </si>
+  <si>
+    <t>OLAKANMI-NOBLE, OLUWAFUNKE FRANCISCA</t>
+  </si>
+  <si>
+    <t>AKINGBADE, ABIODUN</t>
+  </si>
+  <si>
+    <t>HAMMA, IBRAHIM</t>
+  </si>
+  <si>
+    <t>EMMANUEL, ADEBOBOLA SUNDAY</t>
+  </si>
+  <si>
+    <t>ORABUCHE, COLLINS IKECHUKWU</t>
+  </si>
+  <si>
+    <t>INIKA, BAM EKO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DEJI ESAN </t>
+  </si>
+  <si>
+    <t>Abdulwasiu AJETUNMOBI</t>
+  </si>
+  <si>
+    <t>POLLYN, GABRIEL ABINYE</t>
+  </si>
+  <si>
+    <t>ATSU-ABUATO, JULIET</t>
+  </si>
+  <si>
+    <t>YAKUBU, MUHAMMAD MUSTAPHA</t>
+  </si>
+  <si>
+    <t>KUNDE, ALI</t>
+  </si>
+  <si>
+    <t>ONABAJO, ADESEGUN OLATUNBOSUN</t>
+  </si>
+  <si>
+    <t>EKPO, OKON MOSES</t>
+  </si>
+  <si>
+    <t>ADELEYE, OLATUNJI ADEDEJI</t>
+  </si>
+  <si>
+    <t>JAMES, NSIDIETI VICTOR</t>
+  </si>
+  <si>
+    <t>IWUEZE-IFEANYI, CHIDINMA JOY</t>
+  </si>
+  <si>
+    <t>MELA, DIO MELA</t>
+  </si>
+  <si>
+    <t>AGBAJE, ABUBAKAR SEGUN</t>
+  </si>
+  <si>
+    <t>MITAIRE, ONAVWIE EMMANUEL</t>
+  </si>
+  <si>
+    <t>ESSIEN, EKPENYONG EFFIOM</t>
+  </si>
+  <si>
+    <t>OKUTACHI, PETER AROME</t>
+  </si>
+  <si>
+    <t>UYOK, IDARA ALBERT</t>
+  </si>
+  <si>
+    <t>SALAM, ADEYINKA LUKEMAN</t>
+  </si>
+  <si>
+    <t>INYANG, INYANG BASSEY</t>
+  </si>
+  <si>
+    <t>EBADAN, PHILLIAN AKHERE</t>
+  </si>
+  <si>
+    <t>FABIYI, OLUWASEUN MOSES</t>
+  </si>
+  <si>
+    <t>ALAKA, LATEEF BABATUNDE</t>
+  </si>
+  <si>
+    <t>STEPHEN DARAMOLA</t>
+  </si>
+  <si>
+    <t>ALIMI, OLANIYI RAUF</t>
+  </si>
+  <si>
+    <t>OSSAI OPUTE, SANDRA CHINEDU</t>
+  </si>
+  <si>
+    <t>AINA, OLUWATOSIN ADEOLA</t>
   </si>
 </sst>
 </file>
@@ -328,7 +538,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -362,6 +572,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -423,11 +639,8 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -438,8 +651,15 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -724,10 +944,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B82"/>
+  <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B82"/>
+    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
+      <selection activeCell="A83" sqref="A83:B165"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -737,54 +957,54 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="8">
+      <c r="A1" s="7">
         <v>1</v>
       </c>
-      <c r="B1" s="8"/>
+      <c r="B1" s="7"/>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3" s="1"/>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="B5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
@@ -795,577 +1015,1228 @@
       <c r="B8" s="9"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" s="2" t="s">
+      <c r="A11" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" s="2" t="s">
+      <c r="A14" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="2" t="s">
+      <c r="B14" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="1">
+      <c r="A15" s="8">
         <v>3</v>
       </c>
-      <c r="B15" s="1"/>
+      <c r="B15" s="8"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A16" s="2" t="s">
+      <c r="A16" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="2" t="s">
+      <c r="B16" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A17" s="4" t="s">
+      <c r="A17" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B17" s="2" t="s">
+      <c r="B17" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="5" t="s">
         <v>24</v>
       </c>
-      <c r="B18" s="2" t="s">
+      <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A19" s="6" t="s">
+      <c r="A19" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="2" t="s">
+      <c r="B19" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A20" s="4" t="s">
+      <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="2" t="s">
+      <c r="B20" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A21" s="2" t="s">
+      <c r="A21" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="2" t="s">
+      <c r="B21" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="1">
+      <c r="A22" s="8">
         <v>4</v>
       </c>
-      <c r="B22" s="1"/>
+      <c r="B22" s="8"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A23" s="6" t="s">
+      <c r="A23" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="B23" s="2" t="s">
+      <c r="B23" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A24" s="6" t="s">
+      <c r="A24" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="B24" s="2" t="s">
+      <c r="B24" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A25" s="2" t="s">
+      <c r="A25" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B25" s="2" t="s">
+      <c r="B25" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A26" s="2" t="s">
+      <c r="A26" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B26" s="2" t="s">
+      <c r="B26" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A27" s="2" t="s">
+      <c r="A27" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B27" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A28" s="2" t="s">
+      <c r="A28" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B28" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="1">
+      <c r="A29" s="8">
         <v>5</v>
       </c>
-      <c r="B29" s="1"/>
+      <c r="B29" s="8"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A30" s="6" t="s">
+      <c r="A30" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="B30" s="2" t="s">
+      <c r="B30" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A31" s="2" t="s">
+      <c r="A31" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="B31" s="2" t="s">
+      <c r="B31" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A32" s="6" t="s">
+      <c r="A32" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="B32" s="2" t="s">
+      <c r="B32" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A33" s="6" t="s">
+      <c r="A33" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="B33" s="2" t="s">
+      <c r="B33" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B34" s="2" t="s">
+      <c r="B34" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A35" s="6" t="s">
+      <c r="A35" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="B35" s="2" t="s">
+      <c r="B35" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="1">
+      <c r="A36" s="8">
         <v>6</v>
       </c>
-      <c r="B36" s="1"/>
+      <c r="B36" s="8"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A37" s="2" t="s">
+      <c r="A37" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B37" s="2" t="s">
+      <c r="B37" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A38" s="2" t="s">
+      <c r="A38" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B38" s="2" t="s">
+      <c r="B38" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A39" s="2" t="s">
+      <c r="A39" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="B39" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A40" s="2" t="s">
+      <c r="A40" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B40" s="2" t="s">
+      <c r="B40" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A41" s="2" t="s">
+      <c r="A41" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B41" s="2" t="s">
+      <c r="B41" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="1">
+      <c r="A42" s="8">
         <v>7</v>
       </c>
-      <c r="B42" s="1"/>
+      <c r="B42" s="8"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A43" s="2" t="s">
+      <c r="A43" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B43" s="2" t="s">
+      <c r="B43" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A44" s="2" t="s">
+      <c r="A44" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B44" s="2" t="s">
+      <c r="B44" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A45" s="7" t="s">
+      <c r="A45" s="6" t="s">
         <v>51</v>
       </c>
-      <c r="B45" s="2" t="s">
+      <c r="B45" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A46" s="2" t="s">
+      <c r="A46" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="B46" s="2" t="s">
+      <c r="B46" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A47" s="7" t="s">
+      <c r="A47" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="B47" s="2" t="s">
+      <c r="B47" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="1">
+      <c r="A48" s="8">
         <v>8</v>
       </c>
-      <c r="B48" s="1"/>
+      <c r="B48" s="8"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A49" s="2" t="s">
+      <c r="A49" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="B49" s="2" t="s">
+      <c r="B49" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A50" s="2" t="s">
+      <c r="A50" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B50" s="2" t="s">
+      <c r="B50" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A51" s="2" t="s">
+      <c r="A51" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B51" s="2" t="s">
+      <c r="B51" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A52" s="2" t="s">
+      <c r="A52" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="B52" s="2" t="s">
+      <c r="B52" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A53" s="2" t="s">
+      <c r="A53" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="B53" s="2" t="s">
+      <c r="B53" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="1">
+      <c r="A54" s="8">
         <v>9</v>
       </c>
-      <c r="B54" s="1"/>
+      <c r="B54" s="8"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A55" s="2" t="s">
+      <c r="A55" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="B55" s="2" t="s">
+      <c r="B55" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A56" s="2" t="s">
+      <c r="A56" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="2" t="s">
+      <c r="B56" s="1" t="s">
         <v>30</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A57" s="2" t="s">
+      <c r="A57" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="2" t="s">
+      <c r="B57" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A58" s="2" t="s">
+      <c r="A58" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="2" t="s">
+      <c r="B58" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A59" s="2" t="s">
+      <c r="A59" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="2" t="s">
+      <c r="B59" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="1">
+      <c r="A60" s="8">
         <v>10</v>
       </c>
-      <c r="B60" s="1"/>
+      <c r="B60" s="8"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A61" s="2" t="s">
+      <c r="A61" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B61" s="2" t="s">
+      <c r="B61" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A62" s="2" t="s">
+      <c r="A62" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B62" s="2" t="s">
+      <c r="B62" s="1" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A63" s="2" t="s">
+      <c r="A63" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B63" s="2" t="s">
+      <c r="B63" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A64" s="2" t="s">
+      <c r="A64" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="B64" s="2" t="s">
+      <c r="B64" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="1">
+      <c r="A65" s="8">
         <v>11</v>
       </c>
-      <c r="B65" s="1"/>
+      <c r="B65" s="8"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="B66" s="2" t="s">
+      <c r="B66" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="4" t="s">
         <v>69</v>
       </c>
-      <c r="B67" s="2" t="s">
+      <c r="B67" s="1" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A68" s="5" t="s">
+      <c r="A68" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="B68" s="2" t="s">
+      <c r="B68" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A69" s="5" t="s">
+      <c r="A69" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B69" s="2" t="s">
+      <c r="B69" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="1">
+      <c r="A70" s="8">
         <v>12</v>
       </c>
-      <c r="B70" s="1"/>
+      <c r="B70" s="8"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A71" s="2" t="s">
+      <c r="A71" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="B71" s="2" t="s">
+      <c r="B71" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A72" s="2" t="s">
+      <c r="A72" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="B72" s="2" t="s">
+      <c r="B72" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A73" s="2" t="s">
+      <c r="A73" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="B73" s="2" t="s">
+      <c r="B73" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A74" s="2" t="s">
+      <c r="A74" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="B74" s="2" t="s">
+      <c r="B74" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A75" s="2" t="s">
+      <c r="A75" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B75" s="2" t="s">
+      <c r="B75" s="1" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A76" s="2" t="s">
+      <c r="A76" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="B76" s="2" t="s">
+      <c r="B76" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="1">
+      <c r="A77" s="8">
         <v>13</v>
       </c>
-      <c r="B77" s="1"/>
+      <c r="B77" s="8"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A78" s="2" t="s">
+      <c r="A78" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="B78" s="2" t="s">
+      <c r="B78" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A79" s="3" t="s">
+      <c r="A79" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="B79" s="3" t="s">
+      <c r="B79" s="2" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A80" s="2" t="s">
+      <c r="A80" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="B80" s="2" t="s">
+      <c r="B80" s="1" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A81" s="2" t="s">
+      <c r="A81" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="B81" s="2" t="s">
+      <c r="B81" s="1" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A82" s="2" t="s">
+      <c r="A82" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="B82" s="2" t="s">
+      <c r="B82" s="1" t="s">
         <v>40</v>
       </c>
     </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A83" s="8">
+        <v>14</v>
+      </c>
+      <c r="B83" s="8"/>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A84" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="B84" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A85" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B85" s="11" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A86" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="B86" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A87" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="B87" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A88" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="B88" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A89" s="8">
+        <v>15</v>
+      </c>
+      <c r="B89" s="8"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" s="10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="B94" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="8">
+        <v>16</v>
+      </c>
+      <c r="B95" s="8"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="13" t="s">
+        <v>94</v>
+      </c>
+      <c r="B97" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="8">
+        <v>17</v>
+      </c>
+      <c r="B100" s="8"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="B101" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="B102" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="B103" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="B104" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="8">
+        <v>18</v>
+      </c>
+      <c r="B106" s="8"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="B108" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="B109" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="11" t="s">
+        <v>105</v>
+      </c>
+      <c r="B110" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="8">
+        <v>19</v>
+      </c>
+      <c r="B112" s="8"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="B113" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B114" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="B115" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="B116" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="11" t="s">
+        <v>111</v>
+      </c>
+      <c r="B117" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="11" t="s">
+        <v>112</v>
+      </c>
+      <c r="B118" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" s="8">
+        <v>20</v>
+      </c>
+      <c r="B119" s="8"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="B120" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" s="11" t="s">
+        <v>114</v>
+      </c>
+      <c r="B121" s="11" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="B122" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" s="11" t="s">
+        <v>116</v>
+      </c>
+      <c r="B123" s="11" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" s="11" t="s">
+        <v>117</v>
+      </c>
+      <c r="B124" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" s="11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B125" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="8">
+        <v>21</v>
+      </c>
+      <c r="B126" s="8"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="11" t="s">
+        <v>119</v>
+      </c>
+      <c r="B127" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="B128" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" s="11" t="s">
+        <v>121</v>
+      </c>
+      <c r="B129" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" s="11" t="s">
+        <v>122</v>
+      </c>
+      <c r="B130" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" s="11" t="s">
+        <v>123</v>
+      </c>
+      <c r="B131" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" s="8">
+        <v>22</v>
+      </c>
+      <c r="B132" s="8"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" s="11" t="s">
+        <v>124</v>
+      </c>
+      <c r="B133" s="11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" s="11" t="s">
+        <v>125</v>
+      </c>
+      <c r="B134" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" s="11" t="s">
+        <v>126</v>
+      </c>
+      <c r="B135" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" s="12" t="s">
+        <v>127</v>
+      </c>
+      <c r="B136" s="11" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" s="11" t="s">
+        <v>128</v>
+      </c>
+      <c r="B137" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" s="11" t="s">
+        <v>129</v>
+      </c>
+      <c r="B138" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" s="8">
+        <v>23</v>
+      </c>
+      <c r="B139" s="8"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" s="11" t="s">
+        <v>130</v>
+      </c>
+      <c r="B140" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="12" t="s">
+        <v>131</v>
+      </c>
+      <c r="B141" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" s="11" t="s">
+        <v>132</v>
+      </c>
+      <c r="B142" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" s="11" t="s">
+        <v>133</v>
+      </c>
+      <c r="B143" s="11" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B144" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" s="11" t="s">
+        <v>135</v>
+      </c>
+      <c r="B145" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" s="8">
+        <v>24</v>
+      </c>
+      <c r="B146" s="8"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" s="11" t="s">
+        <v>136</v>
+      </c>
+      <c r="B147" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" s="11" t="s">
+        <v>137</v>
+      </c>
+      <c r="B148" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" s="11" t="s">
+        <v>138</v>
+      </c>
+      <c r="B149" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" s="12" t="s">
+        <v>139</v>
+      </c>
+      <c r="B150" s="12" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" s="11" t="s">
+        <v>140</v>
+      </c>
+      <c r="B151" s="11" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" s="11" t="s">
+        <v>141</v>
+      </c>
+      <c r="B152" s="11" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" s="8">
+        <v>25</v>
+      </c>
+      <c r="B153" s="8"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="11" t="s">
+        <v>142</v>
+      </c>
+      <c r="B154" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" s="11" t="s">
+        <v>143</v>
+      </c>
+      <c r="B155" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="B156" s="11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B157" s="11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" s="11" t="s">
+        <v>146</v>
+      </c>
+      <c r="B158" s="11" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" s="12" t="s">
+        <v>147</v>
+      </c>
+      <c r="B159" s="12" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" s="8">
+        <v>26</v>
+      </c>
+      <c r="B160" s="8"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="B161" s="11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="B162" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="B163" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" s="12" t="s">
+        <v>151</v>
+      </c>
+      <c r="B164" s="12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="165" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A165" s="11" t="s">
+        <v>152</v>
+      </c>
+      <c r="B165" s="11" t="s">
+        <v>17</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="25">
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A100:B100"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A146:B146"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A36:B36"/>

</xml_diff>

<commit_message>
Tables updated on the sitting arrangement sheet
</commit_message>
<xml_diff>
--- a/static/seating.xlsx
+++ b/static/seating.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="153">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="303" uniqueCount="179">
   <si>
     <t>ALADE-AKINYEMI, LOLU</t>
   </si>
@@ -483,6 +483,84 @@
   </si>
   <si>
     <t>AINA, OLUWATOSIN ADEOLA</t>
+  </si>
+  <si>
+    <t>Table 1</t>
+  </si>
+  <si>
+    <t>Table 2</t>
+  </si>
+  <si>
+    <t>Table 3</t>
+  </si>
+  <si>
+    <t>Table 4</t>
+  </si>
+  <si>
+    <t>Table 5</t>
+  </si>
+  <si>
+    <t>Table 6</t>
+  </si>
+  <si>
+    <t>Table 7</t>
+  </si>
+  <si>
+    <t>Table 8</t>
+  </si>
+  <si>
+    <t>Table 9</t>
+  </si>
+  <si>
+    <t>Table 10</t>
+  </si>
+  <si>
+    <t>Table 11</t>
+  </si>
+  <si>
+    <t>Table 12</t>
+  </si>
+  <si>
+    <t>Table 13</t>
+  </si>
+  <si>
+    <t>Table 14</t>
+  </si>
+  <si>
+    <t>Table 15</t>
+  </si>
+  <si>
+    <t>Table 16</t>
+  </si>
+  <si>
+    <t>Table 17</t>
+  </si>
+  <si>
+    <t>Table 18</t>
+  </si>
+  <si>
+    <t>Table 19</t>
+  </si>
+  <si>
+    <t>Table 20</t>
+  </si>
+  <si>
+    <t>Table 21</t>
+  </si>
+  <si>
+    <t>Table 22</t>
+  </si>
+  <si>
+    <t>Table 23</t>
+  </si>
+  <si>
+    <t>Table 24</t>
+  </si>
+  <si>
+    <t>Table 25</t>
+  </si>
+  <si>
+    <t>Table 26</t>
   </si>
 </sst>
 </file>
@@ -650,16 +728,16 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="5">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,8 +1024,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B165"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A154" workbookViewId="0">
-      <selection activeCell="A83" sqref="A83:B165"/>
+    <sheetView tabSelected="1" topLeftCell="A135" workbookViewId="0">
+      <selection activeCell="C153" sqref="C153"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -957,8 +1035,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A1" s="7">
-        <v>1</v>
+      <c r="A1" s="7" t="s">
+        <v>153</v>
       </c>
       <c r="B1" s="7"/>
     </row>
@@ -1009,10 +1087,10 @@
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" s="9">
-        <v>2</v>
-      </c>
-      <c r="B8" s="9"/>
+      <c r="A8" s="13" t="s">
+        <v>154</v>
+      </c>
+      <c r="B8" s="13"/>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
@@ -1063,10 +1141,10 @@
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A15" s="8">
-        <v>3</v>
-      </c>
-      <c r="B15" s="8"/>
+      <c r="A15" s="12" t="s">
+        <v>155</v>
+      </c>
+      <c r="B15" s="12"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
@@ -1117,10 +1195,10 @@
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A22" s="8">
-        <v>4</v>
-      </c>
-      <c r="B22" s="8"/>
+      <c r="A22" s="12" t="s">
+        <v>156</v>
+      </c>
+      <c r="B22" s="12"/>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A23" s="5" t="s">
@@ -1171,10 +1249,10 @@
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A29" s="8">
-        <v>5</v>
-      </c>
-      <c r="B29" s="8"/>
+      <c r="A29" s="12" t="s">
+        <v>157</v>
+      </c>
+      <c r="B29" s="12"/>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A30" s="5" t="s">
@@ -1225,10 +1303,10 @@
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A36" s="8">
-        <v>6</v>
-      </c>
-      <c r="B36" s="8"/>
+      <c r="A36" s="12" t="s">
+        <v>158</v>
+      </c>
+      <c r="B36" s="12"/>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
@@ -1271,10 +1349,10 @@
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A42" s="8">
-        <v>7</v>
-      </c>
-      <c r="B42" s="8"/>
+      <c r="A42" s="12" t="s">
+        <v>159</v>
+      </c>
+      <c r="B42" s="12"/>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
@@ -1317,10 +1395,10 @@
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A48" s="8">
-        <v>8</v>
-      </c>
-      <c r="B48" s="8"/>
+      <c r="A48" s="12" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" s="12"/>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
@@ -1363,10 +1441,10 @@
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A54" s="8">
-        <v>9</v>
-      </c>
-      <c r="B54" s="8"/>
+      <c r="A54" s="12" t="s">
+        <v>161</v>
+      </c>
+      <c r="B54" s="12"/>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
@@ -1409,10 +1487,10 @@
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A60" s="8">
-        <v>10</v>
-      </c>
-      <c r="B60" s="8"/>
+      <c r="A60" s="12" t="s">
+        <v>162</v>
+      </c>
+      <c r="B60" s="12"/>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
@@ -1447,10 +1525,10 @@
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A65" s="8">
-        <v>11</v>
-      </c>
-      <c r="B65" s="8"/>
+      <c r="A65" s="12" t="s">
+        <v>163</v>
+      </c>
+      <c r="B65" s="12"/>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A66" s="4" t="s">
@@ -1485,10 +1563,10 @@
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A70" s="8">
-        <v>12</v>
-      </c>
-      <c r="B70" s="8"/>
+      <c r="A70" s="12" t="s">
+        <v>164</v>
+      </c>
+      <c r="B70" s="12"/>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
@@ -1539,10 +1617,10 @@
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A77" s="8">
-        <v>13</v>
-      </c>
-      <c r="B77" s="8"/>
+      <c r="A77" s="12" t="s">
+        <v>165</v>
+      </c>
+      <c r="B77" s="12"/>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
@@ -1585,658 +1663,645 @@
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A83" s="8">
-        <v>14</v>
-      </c>
-      <c r="B83" s="8"/>
+      <c r="A83" s="12" t="s">
+        <v>166</v>
+      </c>
+      <c r="B83" s="12"/>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A84" s="11" t="s">
+      <c r="A84" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="B84" s="11" t="s">
+      <c r="B84" s="9" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A85" s="11" t="s">
+      <c r="A85" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="B85" s="11" t="s">
+      <c r="B85" s="9" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A86" s="11" t="s">
+      <c r="A86" s="9" t="s">
         <v>85</v>
       </c>
-      <c r="B86" s="11" t="s">
+      <c r="B86" s="9" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A87" s="11" t="s">
+      <c r="A87" s="9" t="s">
         <v>86</v>
       </c>
-      <c r="B87" s="11" t="s">
+      <c r="B87" s="9" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A88" s="11" t="s">
+      <c r="A88" s="9" t="s">
         <v>87</v>
       </c>
-      <c r="B88" s="11" t="s">
+      <c r="B88" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A89" s="8">
+      <c r="A89" s="12" t="s">
+        <v>167</v>
+      </c>
+      <c r="B89" s="12"/>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A90" s="9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B90" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A91" s="9" t="s">
+        <v>89</v>
+      </c>
+      <c r="B91" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A92" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="B92" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A93" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="B93" s="8" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A94" s="9" t="s">
+        <v>92</v>
+      </c>
+      <c r="B94" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A95" s="12" t="s">
+        <v>168</v>
+      </c>
+      <c r="B95" s="12"/>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A96" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="B96" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A97" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="B97" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A98" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="B98" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A99" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="B99" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A100" s="12" t="s">
+        <v>169</v>
+      </c>
+      <c r="B100" s="12"/>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A101" s="9" t="s">
+        <v>97</v>
+      </c>
+      <c r="B101" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A102" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="B102" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A103" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="B103" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A104" s="9" t="s">
+        <v>100</v>
+      </c>
+      <c r="B104" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A105" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="B105" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="12" t="s">
+        <v>170</v>
+      </c>
+      <c r="B106" s="12"/>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A107" s="9" t="s">
+        <v>102</v>
+      </c>
+      <c r="B107" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A108" s="9" t="s">
+        <v>103</v>
+      </c>
+      <c r="B108" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A109" s="9" t="s">
+        <v>104</v>
+      </c>
+      <c r="B109" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A110" s="9" t="s">
+        <v>105</v>
+      </c>
+      <c r="B110" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B89" s="8"/>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A90" s="11" t="s">
-        <v>88</v>
-      </c>
-      <c r="B90" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A91" s="11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B91" s="11" t="s">
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A111" s="9" t="s">
+        <v>106</v>
+      </c>
+      <c r="B111" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A112" s="12" t="s">
+        <v>171</v>
+      </c>
+      <c r="B112" s="12"/>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A113" s="9" t="s">
+        <v>107</v>
+      </c>
+      <c r="B113" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A114" s="9" t="s">
+        <v>108</v>
+      </c>
+      <c r="B114" s="9" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A115" s="9" t="s">
+        <v>109</v>
+      </c>
+      <c r="B115" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A116" s="9" t="s">
+        <v>110</v>
+      </c>
+      <c r="B116" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A117" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="B117" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A118" s="9" t="s">
+        <v>112</v>
+      </c>
+      <c r="B118" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A119" s="12" t="s">
+        <v>172</v>
+      </c>
+      <c r="B119" s="12"/>
+    </row>
+    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A120" s="9" t="s">
+        <v>113</v>
+      </c>
+      <c r="B120" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A121" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="B121" s="9" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A122" s="9" t="s">
+        <v>115</v>
+      </c>
+      <c r="B122" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A123" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B123" s="9" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A124" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="B124" s="9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A92" s="11" t="s">
-        <v>90</v>
-      </c>
-      <c r="B92" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A93" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="B93" s="10" t="s">
+    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A125" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="B125" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A126" s="12" t="s">
+        <v>173</v>
+      </c>
+      <c r="B126" s="12"/>
+    </row>
+    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A127" s="9" t="s">
+        <v>119</v>
+      </c>
+      <c r="B127" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A128" s="9" t="s">
+        <v>120</v>
+      </c>
+      <c r="B128" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A129" s="9" t="s">
+        <v>121</v>
+      </c>
+      <c r="B129" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A130" s="9" t="s">
+        <v>122</v>
+      </c>
+      <c r="B130" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A131" s="9" t="s">
+        <v>123</v>
+      </c>
+      <c r="B131" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A132" s="12" t="s">
+        <v>174</v>
+      </c>
+      <c r="B132" s="12"/>
+    </row>
+    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A133" s="9" t="s">
+        <v>124</v>
+      </c>
+      <c r="B133" s="9" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A134" s="9" t="s">
+        <v>125</v>
+      </c>
+      <c r="B134" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A135" s="9" t="s">
+        <v>126</v>
+      </c>
+      <c r="B135" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A136" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="B136" s="9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A137" s="9" t="s">
+        <v>128</v>
+      </c>
+      <c r="B137" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A138" s="9" t="s">
+        <v>129</v>
+      </c>
+      <c r="B138" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A139" s="12" t="s">
+        <v>175</v>
+      </c>
+      <c r="B139" s="12"/>
+    </row>
+    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A140" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="B140" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A141" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="B141" s="10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A142" s="9" t="s">
+        <v>132</v>
+      </c>
+      <c r="B142" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A143" s="9" t="s">
+        <v>133</v>
+      </c>
+      <c r="B143" s="9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A144" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="B144" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A145" s="9" t="s">
+        <v>135</v>
+      </c>
+      <c r="B145" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A146" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="B146" s="12"/>
+    </row>
+    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A147" s="9" t="s">
+        <v>136</v>
+      </c>
+      <c r="B147" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A148" s="9" t="s">
+        <v>137</v>
+      </c>
+      <c r="B148" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A149" s="9" t="s">
+        <v>138</v>
+      </c>
+      <c r="B149" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A150" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="B150" s="10" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A151" s="9" t="s">
+        <v>140</v>
+      </c>
+      <c r="B151" s="9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A152" s="9" t="s">
+        <v>141</v>
+      </c>
+      <c r="B152" s="9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A153" s="12" t="s">
+        <v>177</v>
+      </c>
+      <c r="B153" s="12"/>
+    </row>
+    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A154" s="9" t="s">
+        <v>142</v>
+      </c>
+      <c r="B154" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A155" s="9" t="s">
+        <v>143</v>
+      </c>
+      <c r="B155" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A156" s="9" t="s">
+        <v>144</v>
+      </c>
+      <c r="B156" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A157" s="9" t="s">
+        <v>145</v>
+      </c>
+      <c r="B157" s="9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A158" s="9" t="s">
+        <v>146</v>
+      </c>
+      <c r="B158" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A159" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="B159" s="10" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A160" s="12" t="s">
+        <v>178</v>
+      </c>
+      <c r="B160" s="12"/>
+    </row>
+    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A161" s="9" t="s">
+        <v>148</v>
+      </c>
+      <c r="B161" s="9" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A162" s="9" t="s">
+        <v>149</v>
+      </c>
+      <c r="B162" s="9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A94" s="11" t="s">
-        <v>92</v>
-      </c>
-      <c r="B94" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A95" s="8">
-        <v>16</v>
-      </c>
-      <c r="B95" s="8"/>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A96" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B96" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A97" s="13" t="s">
-        <v>94</v>
-      </c>
-      <c r="B97" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A98" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="B98" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A99" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="B99" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A100" s="8">
-        <v>17</v>
-      </c>
-      <c r="B100" s="8"/>
-    </row>
-    <row r="101" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A101" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="B101" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="102" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A102" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="B102" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A103" s="11" t="s">
-        <v>99</v>
-      </c>
-      <c r="B103" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="11" t="s">
-        <v>100</v>
-      </c>
-      <c r="B104" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="105" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A105" s="11" t="s">
-        <v>101</v>
-      </c>
-      <c r="B105" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A106" s="8">
-        <v>18</v>
-      </c>
-      <c r="B106" s="8"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="11" t="s">
-        <v>102</v>
-      </c>
-      <c r="B107" s="11" t="s">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A163" s="9" t="s">
+        <v>150</v>
+      </c>
+      <c r="B163" s="9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A164" s="10" t="s">
+        <v>151</v>
+      </c>
+      <c r="B164" s="10" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A108" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="B108" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="109" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A109" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="B109" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="110" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A110" s="11" t="s">
-        <v>105</v>
-      </c>
-      <c r="B110" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="111" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A111" s="11" t="s">
-        <v>106</v>
-      </c>
-      <c r="B111" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="112" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A112" s="8">
-        <v>19</v>
-      </c>
-      <c r="B112" s="8"/>
-    </row>
-    <row r="113" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A113" s="11" t="s">
-        <v>107</v>
-      </c>
-      <c r="B113" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="114" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A114" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="B114" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="115" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A115" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="B115" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="116" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A116" s="11" t="s">
-        <v>110</v>
-      </c>
-      <c r="B116" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="117" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A117" s="11" t="s">
-        <v>111</v>
-      </c>
-      <c r="B117" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="118" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A118" s="11" t="s">
-        <v>112</v>
-      </c>
-      <c r="B118" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="119" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A119" s="8">
-        <v>20</v>
-      </c>
-      <c r="B119" s="8"/>
-    </row>
-    <row r="120" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A120" s="11" t="s">
-        <v>113</v>
-      </c>
-      <c r="B120" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="121" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A121" s="11" t="s">
-        <v>114</v>
-      </c>
-      <c r="B121" s="11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="122" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A122" s="11" t="s">
-        <v>115</v>
-      </c>
-      <c r="B122" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="123" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A123" s="11" t="s">
-        <v>116</v>
-      </c>
-      <c r="B123" s="11" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="124" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A124" s="11" t="s">
-        <v>117</v>
-      </c>
-      <c r="B124" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="125" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A125" s="11" t="s">
-        <v>118</v>
-      </c>
-      <c r="B125" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="126" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A126" s="8">
-        <v>21</v>
-      </c>
-      <c r="B126" s="8"/>
-    </row>
-    <row r="127" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A127" s="11" t="s">
-        <v>119</v>
-      </c>
-      <c r="B127" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="128" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A128" s="11" t="s">
-        <v>120</v>
-      </c>
-      <c r="B128" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="129" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A129" s="11" t="s">
-        <v>121</v>
-      </c>
-      <c r="B129" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="130" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A130" s="11" t="s">
-        <v>122</v>
-      </c>
-      <c r="B130" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="131" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A131" s="11" t="s">
-        <v>123</v>
-      </c>
-      <c r="B131" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="132" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A132" s="8">
-        <v>22</v>
-      </c>
-      <c r="B132" s="8"/>
-    </row>
-    <row r="133" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A133" s="11" t="s">
-        <v>124</v>
-      </c>
-      <c r="B133" s="11" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="134" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A134" s="11" t="s">
-        <v>125</v>
-      </c>
-      <c r="B134" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="135" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A135" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="B135" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="136" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A136" s="12" t="s">
-        <v>127</v>
-      </c>
-      <c r="B136" s="11" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="137" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A137" s="11" t="s">
-        <v>128</v>
-      </c>
-      <c r="B137" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="138" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A138" s="11" t="s">
-        <v>129</v>
-      </c>
-      <c r="B138" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="139" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A139" s="8">
-        <v>23</v>
-      </c>
-      <c r="B139" s="8"/>
-    </row>
-    <row r="140" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A140" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="B140" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="141" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A141" s="12" t="s">
-        <v>131</v>
-      </c>
-      <c r="B141" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="142" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A142" s="11" t="s">
-        <v>132</v>
-      </c>
-      <c r="B142" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="143" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A143" s="11" t="s">
-        <v>133</v>
-      </c>
-      <c r="B143" s="11" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="144" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A144" s="11" t="s">
-        <v>134</v>
-      </c>
-      <c r="B144" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A145" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="B145" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A146" s="8">
-        <v>24</v>
-      </c>
-      <c r="B146" s="8"/>
-    </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A147" s="11" t="s">
-        <v>136</v>
-      </c>
-      <c r="B147" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A148" s="11" t="s">
-        <v>137</v>
-      </c>
-      <c r="B148" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A149" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="B149" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A150" s="12" t="s">
-        <v>139</v>
-      </c>
-      <c r="B150" s="12" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A151" s="11" t="s">
-        <v>140</v>
-      </c>
-      <c r="B151" s="11" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A152" s="11" t="s">
-        <v>141</v>
-      </c>
-      <c r="B152" s="11" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A153" s="8">
-        <v>25</v>
-      </c>
-      <c r="B153" s="8"/>
-    </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A154" s="11" t="s">
-        <v>142</v>
-      </c>
-      <c r="B154" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A155" s="11" t="s">
-        <v>143</v>
-      </c>
-      <c r="B155" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A156" s="11" t="s">
-        <v>144</v>
-      </c>
-      <c r="B156" s="11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A157" s="11" t="s">
-        <v>145</v>
-      </c>
-      <c r="B157" s="11" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A158" s="11" t="s">
-        <v>146</v>
-      </c>
-      <c r="B158" s="11" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A159" s="12" t="s">
-        <v>147</v>
-      </c>
-      <c r="B159" s="12" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A160" s="8">
-        <v>26</v>
-      </c>
-      <c r="B160" s="8"/>
-    </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A161" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="B161" s="11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A162" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="B162" s="11" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A163" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="B163" s="11" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A164" s="12" t="s">
-        <v>151</v>
-      </c>
-      <c r="B164" s="12" t="s">
-        <v>1</v>
-      </c>
-    </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A165" s="11" t="s">
+      <c r="A165" s="9" t="s">
         <v>152</v>
       </c>
-      <c r="B165" s="11" t="s">
+      <c r="B165" s="9" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="A106:B106"/>
-    <mergeCell ref="A83:B83"/>
-    <mergeCell ref="A89:B89"/>
-    <mergeCell ref="A95:B95"/>
-    <mergeCell ref="A100:B100"/>
-    <mergeCell ref="A153:B153"/>
-    <mergeCell ref="A160:B160"/>
-    <mergeCell ref="A112:B112"/>
-    <mergeCell ref="A119:B119"/>
-    <mergeCell ref="A126:B126"/>
-    <mergeCell ref="A132:B132"/>
-    <mergeCell ref="A139:B139"/>
-    <mergeCell ref="A146:B146"/>
     <mergeCell ref="A70:B70"/>
     <mergeCell ref="A77:B77"/>
     <mergeCell ref="A36:B36"/>
@@ -2249,6 +2314,19 @@
     <mergeCell ref="A54:B54"/>
     <mergeCell ref="A60:B60"/>
     <mergeCell ref="A65:B65"/>
+    <mergeCell ref="A153:B153"/>
+    <mergeCell ref="A160:B160"/>
+    <mergeCell ref="A112:B112"/>
+    <mergeCell ref="A119:B119"/>
+    <mergeCell ref="A126:B126"/>
+    <mergeCell ref="A132:B132"/>
+    <mergeCell ref="A139:B139"/>
+    <mergeCell ref="A146:B146"/>
+    <mergeCell ref="A106:B106"/>
+    <mergeCell ref="A83:B83"/>
+    <mergeCell ref="A89:B89"/>
+    <mergeCell ref="A95:B95"/>
+    <mergeCell ref="A100:B100"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>